<commit_message>
Pavani Mounika status 20_01_2021
</commit_message>
<xml_diff>
--- a/PavaniMounika/pavani_mounika_status_18-01-2021/pavani_mounika_status_18-01-2021.xlsx
+++ b/PavaniMounika/pavani_mounika_status_18-01-2021/pavani_mounika_status_18-01-2021.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -139,6 +139,9 @@
     <t>Revised OOPS Concepts:
  Class
  Object</t>
+  </si>
+  <si>
+    <t>attended testing Session</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -648,6 +651,9 @@
       <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>